<commit_message>
Update rapports et assets
Rapport de conception final
Assets "lignes" pour documents
</commit_message>
<xml_diff>
--- a/Backlog Mini Tramways.xlsx
+++ b/Backlog Mini Tramways.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubRepos\MiniTramways\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395FFB14-2DF9-47BB-8F94-A1243441AF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1785DA86-D041-4DE4-B612-86C47EE7FCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,29 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>Carte et bâtiments</t>
   </si>
   <si>
-    <t>Initialisation de la carte</t>
-  </si>
-  <si>
-    <t>Apparition des bâtiments</t>
-  </si>
-  <si>
     <t>Transport</t>
   </si>
   <si>
     <t>Création d'une ligne</t>
   </si>
   <si>
-    <t>Obtention des coordonnées des stations départ/arrivée</t>
-  </si>
-  <si>
-    <t>Génération de la ligne et attribution d'un Tramway</t>
-  </si>
-  <si>
     <t>Tramways</t>
   </si>
   <si>
@@ -68,72 +56,18 @@
     <t>Stations</t>
   </si>
   <si>
-    <t>Récupération des bâtiments dans le rayon</t>
-  </si>
-  <si>
     <t>Voyageurs</t>
   </si>
   <si>
     <t>Apparition des voyageurs dans les maisons</t>
   </si>
   <si>
-    <t>Obtention du commerce ou bureau cible</t>
-  </si>
-  <si>
-    <t>Obtention du trajet à emprunter</t>
-  </si>
-  <si>
-    <t>Interaction avec les stations pour suivre le trajet</t>
-  </si>
-  <si>
-    <t>Obtention d'un lieu et d'un type adapté</t>
-  </si>
-  <si>
-    <t>Génération du bâtiment</t>
-  </si>
-  <si>
-    <t>Initialisation de la grille</t>
-  </si>
-  <si>
-    <t>Initialisation de l'affichage</t>
-  </si>
-  <si>
-    <t>Initialisation des zones</t>
-  </si>
-  <si>
     <t>Indispensables</t>
   </si>
   <si>
     <t>Génération de stations aux intersections</t>
   </si>
   <si>
-    <t>Graphisme et design</t>
-  </si>
-  <si>
-    <t>Design des bâtiments</t>
-  </si>
-  <si>
-    <t>Design du fond de la carte</t>
-  </si>
-  <si>
-    <t>Design des stations</t>
-  </si>
-  <si>
-    <t>Design des lignes</t>
-  </si>
-  <si>
-    <t>Design des tramways</t>
-  </si>
-  <si>
-    <t>Design des indicateurs de charge des stations</t>
-  </si>
-  <si>
-    <t>Design des indicateurs de charge</t>
-  </si>
-  <si>
-    <t>Design des indicateurs de cibles</t>
-  </si>
-  <si>
     <t>Génération et IA</t>
   </si>
   <si>
@@ -167,24 +101,15 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Incrémentation du score</t>
-  </si>
-  <si>
     <t>Sauvegarde du record</t>
   </si>
   <si>
     <t>Vitesse de déroulement</t>
   </si>
   <si>
-    <t>Accélérer ou arrêter le temps</t>
-  </si>
-  <si>
     <t>Amélioration d'une station (rayon)</t>
   </si>
   <si>
-    <t>Ajout de voitures à un tramway</t>
-  </si>
-  <si>
     <t>Ajout de tramways à une ligne</t>
   </si>
   <si>
@@ -203,67 +128,142 @@
     <t>Charger une partie depuis un fichier</t>
   </si>
   <si>
-    <t>Initialisation de la fenêtre</t>
-  </si>
-  <si>
-    <t>1:33</t>
-  </si>
-  <si>
-    <t>2:1</t>
-  </si>
-  <si>
-    <t>3:1</t>
-  </si>
-  <si>
-    <t>5:3</t>
-  </si>
-  <si>
-    <t>4:3</t>
-  </si>
-  <si>
-    <t>9:8</t>
-  </si>
-  <si>
-    <t>10:9</t>
-  </si>
-  <si>
-    <t>11:9</t>
-  </si>
-  <si>
-    <t>12:11</t>
-  </si>
-  <si>
-    <t>13:1</t>
-  </si>
-  <si>
-    <t>18:1</t>
-  </si>
-  <si>
-    <t>19:3,5</t>
-  </si>
-  <si>
-    <t>20:9,19,18</t>
-  </si>
-  <si>
-    <t>21:20</t>
-  </si>
-  <si>
-    <t>18:3</t>
-  </si>
-  <si>
-    <t>19:9</t>
-  </si>
-  <si>
-    <t>20:19</t>
-  </si>
-  <si>
-    <t>21:9</t>
-  </si>
-  <si>
-    <t>22:12,21</t>
-  </si>
-  <si>
-    <t>23:22</t>
+    <t>Affichage de la grille</t>
+  </si>
+  <si>
+    <t>Affichage des zones</t>
+  </si>
+  <si>
+    <t>Plusieurs designs par type de bâtiments</t>
+  </si>
+  <si>
+    <t>Génération d'un bâtiment</t>
+  </si>
+  <si>
+    <t>Sélection des coordonnées de départ/arrivée</t>
+  </si>
+  <si>
+    <t>Affichage du rayon au survol</t>
+  </si>
+  <si>
+    <t>Supprimer les stations inutiles automatiquement</t>
+  </si>
+  <si>
+    <t>Suivi du chemin jusqu'à la cible</t>
+  </si>
+  <si>
+    <t>Gestion du score</t>
+  </si>
+  <si>
+    <t>Accélérer le temps</t>
+  </si>
+  <si>
+    <t>Arrêter le temps</t>
+  </si>
+  <si>
+    <t>Création de la ligne et attribution d'un Tramway</t>
+  </si>
+  <si>
+    <t>Affichage du nombre de personnes dans un tram ou une station</t>
+  </si>
+  <si>
+    <t>Calcul de la satisfaction</t>
+  </si>
+  <si>
+    <t>Amélioration d'un wagon (capacité)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -301,18 +301,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -336,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,7 +347,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC90CC32-74CD-4930-AC52-90CD3C0405D5}">
   <dimension ref="A3:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,383 +676,313 @@
     <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="8" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="45.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9" style="8" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="8" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8">
+        <v>31</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+        <v>47</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="E9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="8" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
       <c r="D11" s="8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="8">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="8">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="8" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="8">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="8">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="8">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="8">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
+      <c r="E16" s="1"/>
     </row>
     <row r="23" spans="1:9" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B23" s="9"/>
-      <c r="C23" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" s="9"/>
       <c r="E23" s="7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="7" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>26</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="I24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I25" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="9">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="7" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="8">
-        <v>25</v>
+      <c r="D34" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="E34" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="8">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="I34" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="8">
-        <v>26</v>
+      <c r="D37" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" s="8">
-        <v>30</v>
-      </c>
-      <c r="I37" t="s">
-        <v>53</v>
+        <v>24</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="8">
-        <v>31</v>
+      <c r="H38" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="I38" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="8">
-        <v>32</v>
+        <v>3</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="I39" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="8">
-        <v>27</v>
+      <c r="D40" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="8">
-        <v>28</v>
+      <c r="D41" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="E41" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rapport maquette et assets
</commit_message>
<xml_diff>
--- a/Backlog Mini Tramways.xlsx
+++ b/Backlog Mini Tramways.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubRepos\MiniTramways\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1785DA86-D041-4DE4-B612-86C47EE7FCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505902F2-74EB-4A10-A67B-DF67E9335F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>Carte et bâtiments</t>
   </si>
@@ -176,81 +176,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -260,10 +185,91 @@
     <t>29</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
+    <t>2:1</t>
+  </si>
+  <si>
+    <t>3:2</t>
+  </si>
+  <si>
+    <t>4:1</t>
+  </si>
+  <si>
+    <t>5:4</t>
+  </si>
+  <si>
+    <t>6:5</t>
+  </si>
+  <si>
+    <t>7:5</t>
+  </si>
+  <si>
+    <t>8:5</t>
+  </si>
+  <si>
+    <t>9:5,3</t>
+  </si>
+  <si>
+    <t>10:5</t>
+  </si>
+  <si>
+    <t>11:3</t>
+  </si>
+  <si>
+    <t>13:12</t>
+  </si>
+  <si>
+    <t>14:9</t>
+  </si>
+  <si>
+    <t>15:2</t>
+  </si>
+  <si>
+    <t>16:3</t>
+  </si>
+  <si>
+    <t>17:7</t>
+  </si>
+  <si>
+    <t>18:5</t>
+  </si>
+  <si>
+    <t>19:18</t>
+  </si>
+  <si>
+    <t>20:13</t>
+  </si>
+  <si>
+    <t>21:20</t>
+  </si>
+  <si>
+    <t>22:2</t>
+  </si>
+  <si>
+    <t>23:5</t>
+  </si>
+  <si>
+    <t>24:5</t>
+  </si>
+  <si>
+    <t>25:5</t>
+  </si>
+  <si>
+    <t>26:5</t>
+  </si>
+  <si>
+    <t>30:29</t>
+  </si>
+  <si>
+    <t>31:29</t>
+  </si>
+  <si>
+    <t>12:11,8,9</t>
+  </si>
+  <si>
+    <t>Affichage</t>
+  </si>
+  <si>
+    <t>Zones</t>
   </si>
 </sst>
 </file>
@@ -301,15 +307,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -326,29 +344,197 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,329 +849,472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC90CC32-74CD-4930-AC52-90CD3C0405D5}">
-  <dimension ref="A3:I41"/>
+  <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="45.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9" style="5" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I4" t="s">
+      <c r="G5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="11" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-      <c r="D14" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>36</v>
       </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="7" t="s">
+      <c r="F24" s="23"/>
+      <c r="G24" s="24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D25" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="F25" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="I24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="E26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="F26" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="E27" s="22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:7" s="4" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="25"/>
+      <c r="C34" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="F35" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="20"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="I34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H35" s="8" t="s">
+      <c r="E41" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="I35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="I38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="I39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="E42" s="22" t="s">
         <v>45</v>
       </c>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>